<commit_message>
updated WBI support in calculators
</commit_message>
<xml_diff>
--- a/RR_fuelflow.xlsx
+++ b/RR_fuelflow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="18375" windowHeight="8625"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="18375" windowHeight="8625"/>
   </bookViews>
   <sheets>
     <sheet name="Calculator" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>name</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>Blue items are drop-down selectors. Orange fields are inputs. Only type into the orange fields.</t>
+  </si>
+  <si>
+    <t>SRMFuel</t>
+  </si>
+  <si>
+    <t>Supports stock, CRP and WBI.</t>
   </si>
 </sst>
 </file>
@@ -494,16 +500,16 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="4" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="5" xfId="8" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="3" borderId="5" xfId="8" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="7" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -860,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IR18"/>
+  <dimension ref="A1:IR19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -874,16 +880,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickTop="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>73</v>
       </c>
       <c r="B2"/>
@@ -892,172 +898,179 @@
       <c r="E2"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3"/>
+      <c r="A3" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="5" t="s">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="9">
-        <v>290</v>
-      </c>
-      <c r="C5" s="9">
-        <v>16</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="9">
+        <v>290</v>
+      </c>
+      <c r="C6" s="9">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="6">
-        <f>B5*9.8066</f>
+    <row r="8" spans="1:6">
+      <c r="B8" s="6">
+        <f>B6*9.8066</f>
         <v>2843.9139999999998</v>
       </c>
-      <c r="C7" s="10">
-        <f>C5*1000/B7</f>
+      <c r="C8" s="10">
+        <f>C6*1000/B8</f>
         <v>5.6260491702632365</v>
       </c>
-      <c r="D7" s="10">
-        <f>C5*1000*B7/2</f>
+      <c r="D8" s="10">
+        <f>C6*1000*B8/2</f>
         <v>22751311.999999996</v>
       </c>
-      <c r="E7" s="10">
-        <f>D7/C7</f>
+      <c r="E8" s="10">
+        <f>D8/C8</f>
         <v>4043923.419697999</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:6">
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="20.25" thickBot="1">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:6">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="20.25" thickBot="1">
+      <c r="A11" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" thickTop="1">
-      <c r="A11" s="22" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickTop="1">
+      <c r="A12" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B12" s="11">
         <v>0.45</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C12" s="11">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D12" s="11">
         <v>0</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E12" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="12">
-        <f>IFERROR(VLOOKUP(B12,Database!$A$2:$B$34,2,FALSE),"-")</f>
+      <c r="B14" s="12">
+        <f>IFERROR(VLOOKUP(B13,Database!$A$2:$B$35,2,FALSE),"-")</f>
         <v>5</v>
       </c>
-      <c r="C13" s="12">
-        <f>IFERROR(VLOOKUP(C12,Database!$A$2:$B$34,2,FALSE),"-")</f>
-        <v>5</v>
-      </c>
-      <c r="D13" s="12" t="str">
-        <f>IFERROR(VLOOKUP(D12,Database!$A$2:$B$34,2,FALSE),"-")</f>
+      <c r="C14" s="12" t="str">
+        <f>IFERROR(VLOOKUP(C13,Database!$A$2:$B$35,2,FALSE),"-")</f>
         <v>-</v>
       </c>
-      <c r="E13" s="13">
+      <c r="D14" s="12" t="str">
+        <f>IFERROR(VLOOKUP(D13,Database!$A$2:$B$35,2,FALSE),"-")</f>
+        <v>-</v>
+      </c>
+      <c r="E14" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" thickTop="1">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:6" ht="16.5" thickTop="1">
+      <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="19">
-        <f t="shared" ref="B14:C14" si="0">IFERROR(($C$7/B13)*B11,"-")</f>
+      <c r="B15" s="17">
+        <f t="shared" ref="B15:C15" si="0">IFERROR(($C$8/B14)*B12,"-")</f>
         <v>0.50634442532369128</v>
       </c>
-      <c r="C14" s="19">
-        <f t="shared" si="0"/>
-        <v>0.61886540872895601</v>
-      </c>
-      <c r="D14" s="19" t="str">
-        <f>IFERROR(($C$7/D13)*D11,"-")</f>
+      <c r="C15" s="17" t="str">
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E14" s="19">
-        <f>SUM(B14:D14)*E11</f>
+      <c r="D15" s="17" t="str">
+        <f>IFERROR(($C$8/D14)*D12,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="E15" s="17">
+        <f>SUM(B15:D15)*E12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="5"/>
-    </row>
     <row r="18" spans="1:3">
-      <c r="C18"/>
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>
@@ -1071,9 +1084,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Database!$A$2:$A$34</xm:f>
+            <xm:f>Database!$A$2:$A$35</xm:f>
           </x14:formula1>
-          <xm:sqref>B12:D12</xm:sqref>
+          <xm:sqref>B13:D13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1083,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV34"/>
+  <dimension ref="A1:IV35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1465,6 +1478,18 @@
       </c>
       <c r="C34" s="15">
         <v>4.1000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="14">
+        <f t="shared" ref="B35" si="2">C35*1000</f>
+        <v>7.5</v>
+      </c>
+      <c r="C35" s="15">
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1504,15 +1529,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">

</xml_diff>